<commit_message>
Schematic finished and BOM started
</commit_message>
<xml_diff>
--- a/Documentation/Watch Main BOM.xlsx
+++ b/Documentation/Watch Main BOM.xlsx
@@ -1,29 +1,434 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D3744B-2622-487A-9310-37D5C29CE672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
+  <si>
+    <t xml:space="preserve">DFE201612E-2R2M=P2 </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>VDD11 Buck inductor</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Murata-Electronics/DFE201612E-2R2M%3dP2?qs=AQlKX63v8Rsi4vow61OBVg%3D%3D</t>
+  </si>
+  <si>
+    <t>Passives</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Battery charger, 1V8, 3V3 regulators</t>
+  </si>
+  <si>
+    <t>ADP5360ACBZ-2-R7</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Analog-Devices/ADP5360ACBZ-2-R7?qs=GBLSl2AkirtayaN8yEOC7w%3D%3D</t>
+  </si>
+  <si>
+    <t>ADP5360ACBZ-2-R8</t>
+  </si>
+  <si>
+    <t>FETs</t>
+  </si>
+  <si>
+    <t>DMP2104LP-7</t>
+  </si>
+  <si>
+    <t>Reverse polarity PMOS</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Diodes-Incorporated/DMP2104LP-7?qs=R%252By5Lqt1H6xg6KRllhPj7w%3D%3D</t>
+  </si>
+  <si>
+    <t>ICs</t>
+  </si>
+  <si>
+    <t>DFE201612E-4R7M=P2</t>
+  </si>
+  <si>
+    <t>4.7uH</t>
+  </si>
+  <si>
+    <t>1V8, 3V3 Regulator inductors</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Murata-Electronics/DFE201612E-4R7M%3dP2?qs=AQlKX63v8RtFKyOOIfSFEA%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLZ1608N2R2LT000 </t>
+  </si>
+  <si>
+    <t>1V2 Buck inductor</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TDK/MLZ1608N2R2LT000?qs=%2FPzWLGNeQ%252BiJ52%2F8MHH%252Bdw%3D%3D</t>
+  </si>
+  <si>
+    <t>Inductors</t>
+  </si>
+  <si>
+    <t>Ferrite Beads</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TDK/MAF1005FRQ801AT000?qs=1Kr7Jg1SGW%2Fvot%252BijwBmgw%3D%3D</t>
+  </si>
+  <si>
+    <t>MAF1005FRQ801AT000</t>
+  </si>
+  <si>
+    <t>3V3A Filtering</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>EVP-AEJB2A</t>
+  </si>
+  <si>
+    <t>Side button</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Panasonic/EVP-AEJB2A?qs=WGabLL9VVXqY3HchGWvM%2Fg%3D%3D</t>
+  </si>
+  <si>
+    <t>Bought?</t>
+  </si>
+  <si>
+    <t>4.91mH</t>
+  </si>
+  <si>
+    <t>RFID z-axis transponder coil</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>TR1102-0491J</t>
+  </si>
+  <si>
+    <t>https://www.grupopremo.com/en/tr1102-xy-axis-smd-ferrite-rfid-transponder-inductor-125khz-238-9mh-11x26x22mm/900-tr1102-0491j.html</t>
+  </si>
+  <si>
+    <t>IM70D122V01XTMA1</t>
+  </si>
+  <si>
+    <t>Microphone</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Infineon-Technologies/IM70D122V01XTMA1?qs=8Wlm6%252BaMh8Sl43mQbsC%2FcQ%3D%3D</t>
+  </si>
+  <si>
+    <t>BGA725L6E6327FTSA1</t>
+  </si>
+  <si>
+    <t>GNSS LNA</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Infineon-Technologies/BGA725L6E6327FTSA1?qs=4MqXaUMeF57lT69yR2PUGQ%3D%3D</t>
+  </si>
+  <si>
+    <t>TESEO-LIV3FL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/RF360/B39162B4327P810?qs=lGUynpphgXxwtn5A8O%2FIyg%3D%3D</t>
+  </si>
+  <si>
+    <t>B39162B4327P810</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/TESEO-LIV3FL?qs=sGAEpiMZZMu3sxpa5v1qrtd1MoBwMR%252Bn06QOpIB0k5k%3D</t>
+  </si>
+  <si>
+    <t>GNSS Modile</t>
+  </si>
+  <si>
+    <t>GNSS Saw filter</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TDK/MLZ1608N100LT000?qs=%2FPzWLGNeQ%252BjWztxz0ZUthw%3D%3D</t>
+  </si>
+  <si>
+    <t>4V6, -2V2 Regulator inductors</t>
+  </si>
+  <si>
+    <t>ANT161575TT-3000A1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TDK/ANT161575TT-3000A1?qs=%2FQ2qp2Z%2FWFzXgfHtTXyT%2FQ%3D%3D</t>
+  </si>
+  <si>
+    <t>GNSS + BLE Antenna</t>
+  </si>
+  <si>
+    <t>TPS65631WDSKR</t>
+  </si>
+  <si>
+    <t>4V6, -2V2 Regulator</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Texas-Instruments/TPS65631WDSKR?qs=6E8igxPflKf9wUn%252Bq%252B8X1Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Connectors</t>
+  </si>
+  <si>
+    <t>FH26W-45S-0.3SHW(60)</t>
+  </si>
+  <si>
+    <t>Display connector</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Hirose-Connector/FH26W-45S-0.3SHW60?qs=vcbW%252B4%252BSTIpsVxTSDEXV1Q%3D%3D</t>
+  </si>
+  <si>
+    <t>S26HS512TGABHI000</t>
+  </si>
+  <si>
+    <t>Hyper flash</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Infineon-Technologies/S26HS512TGABHI000?qs=BJlw7L4Cy78X5sI41cfhkg%3D%3D</t>
+  </si>
+  <si>
+    <t>TLV9004SIRTER</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Texas-Instruments/TLV9004SIRTER?qs=byeeYqUIh0P0b6lIyMN1Wg%3D%3D</t>
+  </si>
+  <si>
+    <t>Quad op amp</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Analog-Devices-Maxim-Integrated/MAX9027EBT%2bT?qs=1eQvB6Dk1vgF%252BSfafudw0g%3D%3D</t>
+  </si>
+  <si>
+    <t>MAX9027EBT+T</t>
+  </si>
+  <si>
+    <t>Comparator</t>
+  </si>
+  <si>
+    <t>DMN21D2UFB-7B</t>
+  </si>
+  <si>
+    <t>RFID NMOS</t>
+  </si>
+  <si>
+    <t>DMP21D5UFB4-7B</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Diodes-Incorporated/DMN21D2UFB-7B?qs=gfe7vQ8txpW8IlraWNmMnA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Diodes-Incorporated/DMP21D5UFB4-7B?qs=gfe7vQ8txpUVAcG22XiS3g%3D%3D</t>
+  </si>
+  <si>
+    <t>RFID PMOS</t>
+  </si>
+  <si>
+    <t>Discrete Semis</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>ACDBQC0130L-HF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Comchip-Technology/ACDBQC0130L-HF?qs=Zz7%252BYVVL6bENpHY2DpOUTA%3D%3D</t>
+  </si>
+  <si>
+    <t>RFID Envelope detector diode</t>
+  </si>
+  <si>
+    <t>NVT4858HKZ</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/NXP-Semiconductors/NVT4858HKZ?qs=TuK3vfAjtkUQFuqXj%252BGfyA%3D%3D</t>
+  </si>
+  <si>
+    <t>SD Level shifter</t>
+  </si>
+  <si>
+    <t>105162-0001</t>
+  </si>
+  <si>
+    <t>uSD Card slot</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Molex/105162-0001?qs=1fNsfHe5VsK8daqlgKxZfQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/en/products/detail/panasonic-electric-works/AXG110144A/5057277?s=N4IgTCBcDaIIIA0DiBGFAGFAWLcQF0BfIA</t>
+  </si>
+  <si>
+    <t>AXG110144A</t>
+  </si>
+  <si>
+    <t>LSM6DSO16ISTR</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/LSM6DSO16ISTR?qs=t7xnP681wgUum%252BsoR36hnw%3D%3D</t>
+  </si>
+  <si>
+    <t>OPT3004DNPR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Texas-Instruments/OPT3004DNPR?qs=l7cgNqFNU1jkBuP1vZFGkA%3D%3D</t>
+  </si>
+  <si>
+    <t>Ambient light sensor</t>
+  </si>
+  <si>
+    <t>Magnetometer</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/IIS2MDCTR?qs=1mbolxNpo8ems1K%2FRdQzXg%3D%3D</t>
+  </si>
+  <si>
+    <t>IIS2MDCTR</t>
+  </si>
+  <si>
+    <t>AXG120144A</t>
+  </si>
+  <si>
+    <t>Touch mezzanine socket</t>
+  </si>
+  <si>
+    <t>Lower mezzanine socket</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/en/products/detail/panasonic-electric-works/AXG120144A/5057279</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/STM32U5A9NJH6Q?qs=amGC7iS6iy%252BBZl%252B6aNpvbQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Main MCU</t>
+  </si>
+  <si>
+    <t>STM32U5A9NJH6Q</t>
+  </si>
+  <si>
+    <t>Crystals</t>
+  </si>
+  <si>
+    <t>ECS-.327-7-12-C-TR</t>
+  </si>
+  <si>
+    <t>STM32 LSE</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/ECS/ECS-160-8-37-CWY-TR3?qs=e8oIoAS2J1S7yHPKjK4eXg%3D%3D</t>
+  </si>
+  <si>
+    <t>STM32 HSE</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>ECS-160-8-37-CWY-TR3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/ECS/ECS-.327-7-12-C-TR?qs=Mv7BduZupUigykQeU9laTQ%3D%3D</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +451,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +745,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>14.25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>12.96</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="G15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1.26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1.58</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>5.64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2.46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="G45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G48" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C51" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>59</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>122</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
+        <v>119</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="G55" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="G62" t="s">
+        <v>36</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1.86</v>
+      </c>
+      <c r="G64" t="s">
+        <v>68</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>0.82</v>
+      </c>
+      <c r="G65" t="s">
+        <v>94</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="G66" t="s">
+        <v>108</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>107</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="G67" t="s">
+        <v>109</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F72" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I48" r:id="rId1" xr:uid="{79C09E4D-BADE-4B4A-BEDF-E521AF2CD70D}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{F4A2A264-AC49-480B-919C-77721D13D06A}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{688F96A4-353F-41F2-BDCE-19FB0C4F055C}"/>
+    <hyperlink ref="I41" r:id="rId4" xr:uid="{B2C0CAA1-46A0-4E27-9EB4-036D712BDB7E}"/>
+    <hyperlink ref="I49" r:id="rId5" xr:uid="{E042BE92-CD58-4075-A071-4B3A09485DEE}"/>
+    <hyperlink ref="I50" r:id="rId6" xr:uid="{72003C51-9EB6-4D6C-9A9C-6EEC4EC177AC}"/>
+    <hyperlink ref="I58" r:id="rId7" xr:uid="{82A547C3-62DE-42A5-BDEA-48A9EA696B5A}"/>
+    <hyperlink ref="I62" r:id="rId8" xr:uid="{71B308CD-3568-4BEC-A754-5904C1F26182}"/>
+    <hyperlink ref="I52" r:id="rId9" xr:uid="{BD09006A-42D5-4FE4-BED1-3609604DE8A9}"/>
+    <hyperlink ref="I19" r:id="rId10" xr:uid="{A8D9A3BD-F369-470C-AD04-CFBD40E8EB05}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{923AFC17-08B1-4AD5-AB4A-F49FEEFA3BEC}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{C4894D1D-EE76-4C48-BCEF-A73F596BAA3D}"/>
+    <hyperlink ref="I11" r:id="rId13" xr:uid="{F1E124BF-F8B3-462B-A495-851CF7F46232}"/>
+    <hyperlink ref="I10" r:id="rId14" xr:uid="{0125B906-1A49-48F1-926E-17E98D5F7360}"/>
+    <hyperlink ref="I8" r:id="rId15" xr:uid="{7A3239B6-D0C7-4AF8-98CF-4D888691260D}"/>
+    <hyperlink ref="I64" r:id="rId16" xr:uid="{30E54222-C1AF-4403-9956-97155B7FD8CB}"/>
+    <hyperlink ref="I14" r:id="rId17" xr:uid="{F776EC2B-BBE8-4493-A932-87C91B75736F}"/>
+    <hyperlink ref="I16" r:id="rId18" xr:uid="{9578EC98-BAE7-4517-BA73-440205FB1496}"/>
+    <hyperlink ref="I17" r:id="rId19" xr:uid="{E60881DE-679D-4949-ABE4-1257BB72DA8B}"/>
+    <hyperlink ref="I42" r:id="rId20" xr:uid="{C46E6EAD-628E-4590-9624-4EB11F570573}"/>
+    <hyperlink ref="I43" r:id="rId21" xr:uid="{7813BC07-B2B2-46DA-AF84-F62721CE48AD}"/>
+    <hyperlink ref="I45" r:id="rId22" xr:uid="{B5264A45-0F65-4AA5-8893-2DB67E8ED52C}"/>
+    <hyperlink ref="I15" r:id="rId23" xr:uid="{6530AEEE-15DA-40CC-9C80-56491B7D2AB5}"/>
+    <hyperlink ref="I65" r:id="rId24" xr:uid="{738C619A-46CB-4729-BF40-356AE1BA6342}"/>
+    <hyperlink ref="I66" r:id="rId25" xr:uid="{8E26E8E6-7491-4A28-A0FC-173E24C5257D}"/>
+    <hyperlink ref="I23" r:id="rId26" xr:uid="{354B533E-AE6B-4D10-995D-2E2CE7D75D8A}"/>
+    <hyperlink ref="I25" r:id="rId27" xr:uid="{E88D44C0-FCF9-4D68-914D-FB6014E35C39}"/>
+    <hyperlink ref="I24" r:id="rId28" xr:uid="{D09DD33D-D05C-4448-9139-AD94F4FCFA1B}"/>
+    <hyperlink ref="I67" r:id="rId29" xr:uid="{DF11D2D2-F265-4769-80C5-92206328CB82}"/>
+    <hyperlink ref="I3" r:id="rId30" xr:uid="{767704FF-C400-4F90-B6F1-9D33B5A14B1C}"/>
+    <hyperlink ref="I55" r:id="rId31" xr:uid="{06406781-6B05-4280-99E0-2007222A2286}"/>
+    <hyperlink ref="I54" r:id="rId32" xr:uid="{3D0B6872-F586-4D57-B586-9244EB0BC9CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started routing main PCB
</commit_message>
<xml_diff>
--- a/Documentation/Watch Main BOM.xlsx
+++ b/Documentation/Watch Main BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D3744B-2622-487A-9310-37D5C29CE672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A6640-FB10-4C9D-9B82-F12574F53A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1164" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t xml:space="preserve">DFE201612E-2R2M=P2 </t>
   </si>
@@ -215,9 +215,6 @@
     <t>https://www.mouser.co.uk/ProductDetail/TDK/MLZ1608N100LT000?qs=%2FPzWLGNeQ%252BjWztxz0ZUthw%3D%3D</t>
   </si>
   <si>
-    <t>4V6, -2V2 Regulator inductors</t>
-  </si>
-  <si>
     <t>ANT161575TT-3000A1</t>
   </si>
   <si>
@@ -405,6 +402,30 @@
   </si>
   <si>
     <t>32.768kHz</t>
+  </si>
+  <si>
+    <t>4V6, -2V2, nRF Regulator inductors</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/ECS/ECS-320-8-37B-CWN-TR?qs=3Rah4i%252BhyCHz%252B6r%252BQzq5cA%3D%3D</t>
+  </si>
+  <si>
+    <t>32MHz</t>
+  </si>
+  <si>
+    <t>nRF Oscillator</t>
+  </si>
+  <si>
+    <t>ECS-320-8-37B-CWN-TR</t>
+  </si>
+  <si>
+    <t>nRF5340-QKAA-R7</t>
+  </si>
+  <si>
+    <t>BLE MCU</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Nordic-Semiconductor/nRF5340-QKAA-R7?qs=81r%252BiQLm7BRwq87cqfIJeg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -746,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71:G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +816,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -804,13 +825,30 @@
         <v>14.25</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>7.32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -849,7 +887,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -858,10 +896,10 @@
         <v>1.2</v>
       </c>
       <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -869,7 +907,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -878,10 +916,10 @@
         <v>0.44</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -937,7 +975,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -946,18 +984,18 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -966,15 +1004,15 @@
         <v>0.96</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -983,15 +1021,15 @@
         <v>0.61</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1000,10 +1038,10 @@
         <v>1.26</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.3">
@@ -1037,7 +1075,7 @@
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1046,18 +1084,18 @@
         <v>5.64</v>
       </c>
       <c r="G23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>41</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1066,15 +1104,15 @@
         <v>2.8</v>
       </c>
       <c r="G24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1083,10 +1121,10 @@
         <v>2.46</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1094,7 +1132,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -1117,7 +1155,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -1126,15 +1164,15 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1143,10 +1181,10 @@
         <v>0.3</v>
       </c>
       <c r="G43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1154,10 +1192,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" t="s">
         <v>86</v>
-      </c>
-      <c r="C45" t="s">
-        <v>87</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1166,10 +1204,10 @@
         <v>0.27</v>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1252,13 +1290,13 @@
         <v>56</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F51" s="3">
         <v>0.11</v>
       </c>
       <c r="G51" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>58</v>
@@ -1289,78 +1327,96 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F53" s="3"/>
+      <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
         <v>114</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="G55" t="s">
         <v>115</v>
       </c>
-      <c r="D54" t="s">
-        <v>122</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="G54" t="s">
+      <c r="I55" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="G56" t="s">
+        <v>117</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>120</v>
-      </c>
-      <c r="D55" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="G55" t="s">
-        <v>118</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F57" s="3"/>
+      <c r="C57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" t="s">
+        <v>124</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="G57" t="s">
+        <v>125</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
         <v>29</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>31</v>
       </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
         <v>0.18</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>32</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F60" s="3"/>
@@ -1369,116 +1425,119 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>33</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>34</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>35</v>
       </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" s="3">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
         <v>0.64</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" t="s">
         <v>36</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="I63" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1.86</v>
+      </c>
+      <c r="G65" t="s">
         <v>67</v>
       </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>1.86</v>
-      </c>
-      <c r="G64" t="s">
+      <c r="I65" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0.82</v>
+      </c>
+      <c r="G66" t="s">
         <v>93</v>
       </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>0.82</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="I66" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I65" s="1" t="s">
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="G67" t="s">
+        <v>107</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>97</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="G66" t="s">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>106</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="G68" t="s">
         <v>108</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>107</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67" s="3">
-        <v>2.04</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="I68" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F73" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1489,8 +1548,8 @@
     <hyperlink ref="I41" r:id="rId4" xr:uid="{B2C0CAA1-46A0-4E27-9EB4-036D712BDB7E}"/>
     <hyperlink ref="I49" r:id="rId5" xr:uid="{E042BE92-CD58-4075-A071-4B3A09485DEE}"/>
     <hyperlink ref="I50" r:id="rId6" xr:uid="{72003C51-9EB6-4D6C-9A9C-6EEC4EC177AC}"/>
-    <hyperlink ref="I58" r:id="rId7" xr:uid="{82A547C3-62DE-42A5-BDEA-48A9EA696B5A}"/>
-    <hyperlink ref="I62" r:id="rId8" xr:uid="{71B308CD-3568-4BEC-A754-5904C1F26182}"/>
+    <hyperlink ref="I59" r:id="rId7" xr:uid="{82A547C3-62DE-42A5-BDEA-48A9EA696B5A}"/>
+    <hyperlink ref="I63" r:id="rId8" xr:uid="{71B308CD-3568-4BEC-A754-5904C1F26182}"/>
     <hyperlink ref="I52" r:id="rId9" xr:uid="{BD09006A-42D5-4FE4-BED1-3609604DE8A9}"/>
     <hyperlink ref="I19" r:id="rId10" xr:uid="{A8D9A3BD-F369-470C-AD04-CFBD40E8EB05}"/>
     <hyperlink ref="I12" r:id="rId11" xr:uid="{923AFC17-08B1-4AD5-AB4A-F49FEEFA3BEC}"/>
@@ -1498,7 +1557,7 @@
     <hyperlink ref="I11" r:id="rId13" xr:uid="{F1E124BF-F8B3-462B-A495-851CF7F46232}"/>
     <hyperlink ref="I10" r:id="rId14" xr:uid="{0125B906-1A49-48F1-926E-17E98D5F7360}"/>
     <hyperlink ref="I8" r:id="rId15" xr:uid="{7A3239B6-D0C7-4AF8-98CF-4D888691260D}"/>
-    <hyperlink ref="I64" r:id="rId16" xr:uid="{30E54222-C1AF-4403-9956-97155B7FD8CB}"/>
+    <hyperlink ref="I65" r:id="rId16" xr:uid="{30E54222-C1AF-4403-9956-97155B7FD8CB}"/>
     <hyperlink ref="I14" r:id="rId17" xr:uid="{F776EC2B-BBE8-4493-A932-87C91B75736F}"/>
     <hyperlink ref="I16" r:id="rId18" xr:uid="{9578EC98-BAE7-4517-BA73-440205FB1496}"/>
     <hyperlink ref="I17" r:id="rId19" xr:uid="{E60881DE-679D-4949-ABE4-1257BB72DA8B}"/>
@@ -1506,15 +1565,18 @@
     <hyperlink ref="I43" r:id="rId21" xr:uid="{7813BC07-B2B2-46DA-AF84-F62721CE48AD}"/>
     <hyperlink ref="I45" r:id="rId22" xr:uid="{B5264A45-0F65-4AA5-8893-2DB67E8ED52C}"/>
     <hyperlink ref="I15" r:id="rId23" xr:uid="{6530AEEE-15DA-40CC-9C80-56491B7D2AB5}"/>
-    <hyperlink ref="I65" r:id="rId24" xr:uid="{738C619A-46CB-4729-BF40-356AE1BA6342}"/>
-    <hyperlink ref="I66" r:id="rId25" xr:uid="{8E26E8E6-7491-4A28-A0FC-173E24C5257D}"/>
+    <hyperlink ref="I66" r:id="rId24" xr:uid="{738C619A-46CB-4729-BF40-356AE1BA6342}"/>
+    <hyperlink ref="I67" r:id="rId25" xr:uid="{8E26E8E6-7491-4A28-A0FC-173E24C5257D}"/>
     <hyperlink ref="I23" r:id="rId26" xr:uid="{354B533E-AE6B-4D10-995D-2E2CE7D75D8A}"/>
     <hyperlink ref="I25" r:id="rId27" xr:uid="{E88D44C0-FCF9-4D68-914D-FB6014E35C39}"/>
     <hyperlink ref="I24" r:id="rId28" xr:uid="{D09DD33D-D05C-4448-9139-AD94F4FCFA1B}"/>
-    <hyperlink ref="I67" r:id="rId29" xr:uid="{DF11D2D2-F265-4769-80C5-92206328CB82}"/>
+    <hyperlink ref="I68" r:id="rId29" xr:uid="{DF11D2D2-F265-4769-80C5-92206328CB82}"/>
     <hyperlink ref="I3" r:id="rId30" xr:uid="{767704FF-C400-4F90-B6F1-9D33B5A14B1C}"/>
-    <hyperlink ref="I55" r:id="rId31" xr:uid="{06406781-6B05-4280-99E0-2007222A2286}"/>
-    <hyperlink ref="I54" r:id="rId32" xr:uid="{3D0B6872-F586-4D57-B586-9244EB0BC9CA}"/>
+    <hyperlink ref="I56" r:id="rId31" xr:uid="{06406781-6B05-4280-99E0-2007222A2286}"/>
+    <hyperlink ref="I55" r:id="rId32" xr:uid="{3D0B6872-F586-4D57-B586-9244EB0BC9CA}"/>
+    <hyperlink ref="I51" r:id="rId33" xr:uid="{D440671E-DDBF-432C-9599-F06EDF3BD0EB}"/>
+    <hyperlink ref="I57" r:id="rId34" xr:uid="{C9E51835-D777-4C8A-8B6D-79598CB9D90D}"/>
+    <hyperlink ref="I4" r:id="rId35" xr:uid="{6C239A98-5AD8-44E7-8B22-0BEE5936F859}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New display, started PCB revision 2
</commit_message>
<xml_diff>
--- a/Documentation/Watch Main BOM.xlsx
+++ b/Documentation/Watch Main BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A6640-FB10-4C9D-9B82-F12574F53A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101A7DB2-0E9C-4D20-AA13-D34FF86D9664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1164" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -770,7 +770,7 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E71" sqref="E71:G73"/>
     </sheetView>
   </sheetViews>

</xml_diff>